<commit_message>
Ajout en cours d'icônes
</commit_message>
<xml_diff>
--- a/web/tasks.xlsx
+++ b/web/tasks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="134">
   <si>
     <t>Nom de la class</t>
   </si>
@@ -373,13 +373,61 @@
   </si>
   <si>
     <t>Changer la table renter</t>
+  </si>
+  <si>
+    <t>User:</t>
+  </si>
+  <si>
+    <t>Voir les livres disponibles</t>
+  </si>
+  <si>
+    <t>Annuler une demande d'emprunt</t>
+  </si>
+  <si>
+    <t>Recevoir des alertes qu'il faut rendre le livre</t>
+  </si>
+  <si>
+    <t>Ne peux pas renouveler si un autre utilisateur l'a réservé</t>
+  </si>
+  <si>
+    <t>Renouveler de 7j supp une demande si déjà pris, peut être renouvelé qu'une fois</t>
+  </si>
+  <si>
+    <t>Faire une demande d'emprunt, mis à 2 semaines de base</t>
+  </si>
+  <si>
+    <t>Réserver un livre déjà pris, se met en demande de réservation</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Modifier les livres</t>
+  </si>
+  <si>
+    <t>Accepter des demandes d'emprunt</t>
+  </si>
+  <si>
+    <t>Accepter des demandes de réservation</t>
+  </si>
+  <si>
+    <t>Modifier les utilisateurs sauf soi même</t>
+  </si>
+  <si>
+    <t>Annuler des demandes et réservations</t>
+  </si>
+  <si>
+    <t>Modifier les bibliothèques</t>
+  </si>
+  <si>
+    <t>Reçois une alerte automatique s'il doit rendre un livre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +450,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -413,6 +475,20 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -549,39 +625,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -865,656 +946,657 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D108"/>
+  <dimension ref="A2:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="104.7109375" customWidth="1"/>
-    <col min="4" max="4" width="58.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10" style="3" customWidth="1"/>
+    <col min="3" max="3" width="104.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="58.28515625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="2"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="2"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="B39" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="2"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D41" s="2"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="2"/>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D44" s="2"/>
+      <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D47" s="2"/>
+      <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+      <c r="B48" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="B49" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="2"/>
+      <c r="D49" s="5"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="B50" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="2"/>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="B51" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="2"/>
+      <c r="D51" s="5"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="5"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="B53" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="5"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="B54" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="5"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="B55" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="2"/>
+      <c r="D55" s="5"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="5"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+      <c r="B57" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="5"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="5"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="5"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+      <c r="B60" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="D60" s="5"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D61" s="2"/>
+      <c r="D61" s="5"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D62" s="2"/>
+      <c r="D62" s="5"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D63" s="2"/>
+      <c r="D63" s="5"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D64" s="2"/>
+      <c r="D64" s="5"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D65" s="2"/>
+      <c r="D65" s="5"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D66" s="2"/>
+      <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="2"/>
+      <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D68" s="2"/>
+      <c r="D68" s="5"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D69" s="2"/>
+      <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+      <c r="B70" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D70" s="2"/>
+      <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
     </row>
     <row r="87" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C88" s="9" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="8">
+      <c r="B89" s="10">
         <v>1</v>
       </c>
-      <c r="C89" s="10" t="s">
+      <c r="C89" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="8">
+      <c r="B90" s="10">
         <v>1</v>
       </c>
-      <c r="C90" s="10" t="s">
+      <c r="C90" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="8">
+      <c r="B91" s="10">
         <v>1</v>
       </c>
-      <c r="C91" s="10" t="s">
+      <c r="C91" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="8">
+      <c r="B92" s="10">
         <v>1</v>
       </c>
-      <c r="C92" s="10" t="s">
+      <c r="C92" s="11" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="8">
+      <c r="B93" s="10">
         <v>2</v>
       </c>
-      <c r="C93" s="10" t="s">
+      <c r="C93" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="8">
+      <c r="B94" s="10">
         <v>3</v>
       </c>
-      <c r="C94" s="10" t="s">
+      <c r="C94" s="11" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="8">
+      <c r="B95" s="10">
         <v>3</v>
       </c>
-      <c r="C95" s="10" t="s">
+      <c r="C95" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="96" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="8">
+      <c r="B96" s="10">
         <v>3</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C96" s="11" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="97" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="8">
+      <c r="B97" s="10">
         <v>3</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C97" s="11" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="98" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="8">
+      <c r="B98" s="10">
         <v>3</v>
       </c>
-      <c r="C98" s="10" t="s">
+      <c r="C98" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D98" s="11" t="s">
+      <c r="D98" s="12" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="99" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="8">
+      <c r="B99" s="10">
         <v>4</v>
       </c>
-      <c r="C99" s="10" t="s">
+      <c r="C99" s="11" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="100" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="8">
+      <c r="B100" s="10">
         <v>4</v>
       </c>
-      <c r="C100" s="10" t="s">
+      <c r="C100" s="11" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="101" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="8">
+      <c r="B101" s="10">
         <v>5</v>
       </c>
-      <c r="C101" s="9" t="s">
+      <c r="C101" s="13" t="s">
         <v>106</v>
       </c>
       <c r="D101" s="14" t="s">
@@ -1522,26 +1604,26 @@
       </c>
     </row>
     <row r="102" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="8">
+      <c r="B102" s="10">
         <v>6</v>
       </c>
-      <c r="C102" s="10" t="s">
+      <c r="C102" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="103" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="8">
+      <c r="B103" s="10">
         <v>7</v>
       </c>
-      <c r="C103" s="10" t="s">
+      <c r="C103" s="11" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="104" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="8">
+      <c r="B104" s="10">
         <v>7</v>
       </c>
-      <c r="C104" s="10" t="s">
+      <c r="C104" s="11" t="s">
         <v>109</v>
       </c>
       <c r="D104" s="15" t="s">
@@ -1549,39 +1631,138 @@
       </c>
     </row>
     <row r="105" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="8">
+      <c r="B105" s="10">
         <v>8</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C105" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D105" s="13" t="s">
+      <c r="D105" s="17" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="106" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="8">
+      <c r="B106" s="10">
         <v>9</v>
       </c>
-      <c r="C106" s="12" t="s">
+      <c r="C106" s="18" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="107" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="8">
+      <c r="B107" s="10">
         <v>10</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C107" s="16" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="108" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="8">
+      <c r="B108" s="10">
         <v>11</v>
       </c>
-      <c r="C108" s="7" t="s">
+      <c r="C108" s="16" t="s">
         <v>113</v>
       </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C113" s="2"/>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114" s="2"/>
+      <c r="C114" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115" s="2"/>
+      <c r="C115" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" s="2"/>
+      <c r="C116" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" s="2"/>
+      <c r="C117" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" s="2"/>
+      <c r="C118" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119" s="2"/>
+      <c r="C119" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="2"/>
+      <c r="C120" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B121" s="2"/>
+      <c r="C121" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B123" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C123" s="2"/>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124" s="2"/>
+      <c r="C124" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B125" s="2"/>
+      <c r="C125" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B126" s="2"/>
+      <c r="C126" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B127" s="2"/>
+      <c r="C127" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128" s="2"/>
+      <c r="C128" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" s="2"/>
+      <c r="C129" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>